<commit_message>
Added autolevel options in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>3D PRINTER BOM</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Capacitive proximity sensor</t>
-  </si>
-  <si>
-    <t>Replaces Z endstop *OPTIONAL*</t>
   </si>
   <si>
     <t>Small zip ties</t>
@@ -309,6 +306,15 @@
   </si>
   <si>
     <t>Any type works</t>
+  </si>
+  <si>
+    <t>Pibot Optical Reflection Endstop</t>
+  </si>
+  <si>
+    <t>Replaces Z endstop for autolevel*OPTIONAL*</t>
+  </si>
+  <si>
+    <t>Best option for autolevel, replaces z endstop *OPTIONAL*</t>
   </si>
 </sst>
 </file>
@@ -590,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -642,6 +648,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -947,19 +956,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="71.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="33.75" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="71.75" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,7 +1137,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1278,147 +1287,147 @@
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="32" t="s">
+      <c r="A29" s="47"/>
+      <c r="B29" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="22">
-        <v>1</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B31" s="32" t="s">
         <v>53</v>
-      </c>
-      <c r="C30" s="22">
-        <v>2</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="32" t="s">
-        <v>55</v>
       </c>
       <c r="C31" s="22">
         <v>2</v>
       </c>
-      <c r="D31" s="25" t="s">
-        <v>56</v>
+      <c r="D31" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="22">
         <v>2</v>
       </c>
-      <c r="D32" s="26" t="s">
-        <v>58</v>
+      <c r="D32" s="25" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
       <c r="B33" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C33" s="22">
-        <v>4</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="35"/>
-      <c r="B34" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="42">
+      <c r="B34" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="22">
         <v>4</v>
       </c>
-      <c r="D34" s="43"/>
+      <c r="D34" s="27" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="42">
+        <v>4</v>
+      </c>
+      <c r="D35" s="43"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="46" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="C37" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="36"/>
+      <c r="B39" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="38" t="s">
+      <c r="C39" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+      <c r="D39" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="22" t="s">
         <v>78</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="6">
-        <v>2</v>
-      </c>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="C40" s="6">
         <v>2</v>
@@ -1428,17 +1437,17 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="37"/>
       <c r="B41" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="37"/>
       <c r="B42" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="6">
         <v>1</v>
@@ -1448,7 +1457,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
       <c r="B43" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
@@ -1458,33 +1467,43 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="37"/>
       <c r="B44" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="37"/>
       <c r="B45" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C45" s="6">
+        <v>1</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="37"/>
+      <c r="B46" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="6">
         <v>4</v>
       </c>
-      <c r="D45" s="6"/>
+      <c r="D46" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B34" r:id="rId1"/>
-    <hyperlink ref="B33" r:id="rId2"/>
-    <hyperlink ref="B32" r:id="rId3"/>
-    <hyperlink ref="B31" r:id="rId4"/>
-    <hyperlink ref="B30" r:id="rId5"/>
-    <hyperlink ref="B29" r:id="rId6"/>
+    <hyperlink ref="B35" r:id="rId1"/>
+    <hyperlink ref="B34" r:id="rId2"/>
+    <hyperlink ref="B33" r:id="rId3"/>
+    <hyperlink ref="B32" r:id="rId4"/>
+    <hyperlink ref="B31" r:id="rId5"/>
+    <hyperlink ref="B30" r:id="rId6"/>
     <hyperlink ref="B28" r:id="rId7"/>
     <hyperlink ref="B27" r:id="rId8"/>
     <hyperlink ref="B26" r:id="rId9"/>
@@ -1510,9 +1529,10 @@
     <hyperlink ref="B11" r:id="rId29"/>
     <hyperlink ref="B12" r:id="rId30"/>
     <hyperlink ref="B13" r:id="rId31"/>
+    <hyperlink ref="B29" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="78" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId32"/>
+  <pageSetup scale="78" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId33"/>
 </worksheet>
 </file>
 

</xml_diff>